<commit_message>
update RTM & create IDs to CRS
</commit_message>
<xml_diff>
--- a/Requirements/RTM.xlsx
+++ b/Requirements/RTM.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031E6A21-AA9F-4D59-8DBE-7ADA790BBD7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="52">
   <si>
     <t>SRS</t>
   </si>
@@ -29,9 +28,6 @@
     <t>SIQ</t>
   </si>
   <si>
-    <t>RTM</t>
-  </si>
-  <si>
     <t>SRS_Register_001</t>
   </si>
   <si>
@@ -77,10 +73,6 @@
     <t>SRS_ View Account _001</t>
   </si>
   <si>
-    <t>referenced to 
-High_level_login_1</t>
-  </si>
-  <si>
     <t xml:space="preserve">SRS_ View Account _002          </t>
   </si>
   <si>
@@ -90,14 +82,101 @@
     <t>Low_Design_view_clientAccount_1</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>CRs</t>
+  </si>
+  <si>
+    <t>SRS_Login_004</t>
+  </si>
+  <si>
+    <t>CRs_2.2</t>
+  </si>
+  <si>
+    <t>SRS_Logout_001</t>
+  </si>
+  <si>
+    <t>SRS_Logout_002</t>
+  </si>
+  <si>
+    <t>SRS_Logout_003</t>
+  </si>
+  <si>
+    <t>SRS_PerformTransaction_001</t>
+  </si>
+  <si>
+    <t>SRS_PerformTransaction_002</t>
+  </si>
+  <si>
+    <t>SRS_PerformTransaction_003</t>
+  </si>
+  <si>
+    <t>SRS_PerformTransaction_004</t>
+  </si>
+  <si>
+    <t>SRS_PerformTransaction_005</t>
+  </si>
+  <si>
+    <t>2.2 Login and Logout</t>
+  </si>
+  <si>
+    <t>2.1     Register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.3 View Account </t>
+  </si>
+  <si>
+    <t>2.4 Perform Transaction</t>
+  </si>
+  <si>
+    <t>SRS_AddNewAccount _001</t>
+  </si>
+  <si>
+    <t>2.5 Add New Account</t>
+  </si>
+  <si>
+    <t>2.6 Close Account</t>
+  </si>
+  <si>
+    <t>SRS_Close Account _001</t>
+  </si>
+  <si>
+    <t>SRS_Close. Account _002</t>
+  </si>
+  <si>
+    <t>SRS_Close Account _003</t>
+  </si>
+  <si>
+    <t>High_level_Logout_1</t>
+  </si>
+  <si>
+    <t>High_level_login_admin_1</t>
+  </si>
+  <si>
+    <t>Low_design_add_account_1</t>
+  </si>
+  <si>
+    <t>Low_Design_CloseAccount_1</t>
+  </si>
+  <si>
+    <t>trans_001</t>
+  </si>
+  <si>
+    <t>admin_001</t>
+  </si>
+  <si>
+    <t>CRs_2.1</t>
+  </si>
+  <si>
+    <t>CRs_2.3</t>
+  </si>
+  <si>
+    <t>CRs_1.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,14 +200,8 @@
       <family val="1"/>
       <scheme val="major"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Raleway"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,12 +212,6 @@
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor rgb="FFB4C6E7"/>
       </patternFill>
     </fill>
   </fills>
@@ -172,49 +239,37 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -309,23 +364,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -361,23 +399,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -553,167 +574,458 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="51.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" customWidth="1"/>
-    <col min="3" max="3" width="40.28515625" customWidth="1"/>
-    <col min="4" max="4" width="37.42578125" customWidth="1"/>
+    <col min="1" max="1" width="46.85546875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="39" style="6" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="6" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="7" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="4" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="F2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" s="4" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="E3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" s="2" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="4" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="F4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" s="2" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="4" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="F5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" s="2" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" s="2" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" s="2" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" s="2" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" s="2" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" s="2" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" s="2" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" s="4" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" s="2" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="4" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="4" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" s="4" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-    </row>
-    <row r="13" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-    </row>
-    <row r="14" spans="1:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
+      <c r="F13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:XFD1"/>
+  <mergeCells count="5">
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update as per coach review
</commit_message>
<xml_diff>
--- a/Requirements/RTM.xlsx
+++ b/Requirements/RTM.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED095288-4441-4BEA-8B34-49CFAD5EC3E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="76">
   <si>
     <t>SRS</t>
   </si>
@@ -101,9 +102,6 @@
   </si>
   <si>
     <t>CRs_1.1, CRs_2.2</t>
-  </si>
-  <si>
-    <t>CRs_1.2, CRs_2.4</t>
   </si>
   <si>
     <t>SRS_Login_003</t>
@@ -259,12 +257,15 @@
   <si>
     <t>Class Diagram</t>
   </si>
+  <si>
+    <t xml:space="preserve"> CRs_2.4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -299,6 +300,12 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -390,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -419,6 +426,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -435,12 +451,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -536,6 +546,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -571,6 +598,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -746,12 +790,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="51.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -769,7 +813,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>12</v>
@@ -787,15 +831,15 @@
         <v>1</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>63</v>
+      <c r="A2" s="15" t="s">
+        <v>62</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
@@ -804,20 +848,20 @@
         <v>3</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F2" s="4"/>
-      <c r="G2" s="17" t="s">
-        <v>71</v>
+      <c r="G2" s="11" t="s">
+        <v>70</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
+      <c r="A3" s="16"/>
       <c r="B3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
@@ -827,17 +871,17 @@
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="16"/>
+        <v>47</v>
+      </c>
+      <c r="G3" s="12"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>4</v>
@@ -846,17 +890,17 @@
         <v>6</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F4" s="4"/>
-      <c r="G4" s="16"/>
+      <c r="G4" s="12"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" s="1" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>64</v>
+      <c r="A5" s="17" t="s">
+        <v>63</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>14</v>
@@ -868,18 +912,18 @@
         <v>7</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="G5" s="16" t="s">
-        <v>70</v>
+      <c r="G5" s="12" t="s">
+        <v>69</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="4" t="s">
         <v>28</v>
       </c>
@@ -891,15 +935,15 @@
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="G6" s="16"/>
+        <v>60</v>
+      </c>
+      <c r="G6" s="12"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
@@ -907,19 +951,19 @@
         <v>8</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F7" s="4"/>
-      <c r="G7" s="16"/>
+      <c r="G7" s="12"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
@@ -930,12 +974,12 @@
         <v>13</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="G8" s="16"/>
+        <v>61</v>
+      </c>
+      <c r="G8" s="12"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -949,76 +993,74 @@
         <v>8</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F9" s="4"/>
-      <c r="G9" s="16"/>
+      <c r="G9" s="12"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" s="1" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>65</v>
+      <c r="A10" s="18" t="s">
+        <v>64</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>66</v>
+      <c r="A12" s="14" t="s">
+        <v>65</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>25</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="5"/>
@@ -1026,9 +1068,9 @@
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="4" t="s">
-        <v>29</v>
+      <c r="A13" s="14"/>
+      <c r="B13" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>25</v>
@@ -1037,7 +1079,7 @@
         <v>17</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="5"/>
@@ -1045,18 +1087,16 @@
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="A14" s="14"/>
+      <c r="B14" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="5"/>
@@ -1064,18 +1104,16 @@
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="A15" s="14"/>
+      <c r="B15" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="10"/>
       <c r="D15" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="5"/>
@@ -1083,18 +1121,16 @@
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="A16" s="14"/>
+      <c r="B16" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="10"/>
       <c r="D16" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="5"/>
@@ -1103,17 +1139,15 @@
     </row>
     <row r="17" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
-      <c r="B17" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="B17" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="10"/>
       <c r="D17" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="5"/>
@@ -1122,17 +1156,15 @@
     </row>
     <row r="18" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
-      <c r="B18" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="B18" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="10"/>
       <c r="D18" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="5"/>
@@ -1141,17 +1173,15 @@
     </row>
     <row r="19" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
-      <c r="B19" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="B19" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="10"/>
       <c r="D19" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="5"/>
@@ -1160,10 +1190,10 @@
     </row>
     <row r="20" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
@@ -1172,7 +1202,7 @@
         <v>21</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="5"/>
@@ -1180,11 +1210,11 @@
       <c r="J20" s="5"/>
     </row>
     <row r="21" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
-        <v>68</v>
+      <c r="A21" s="13" t="s">
+        <v>67</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>26</v>
@@ -1193,7 +1223,7 @@
         <v>22</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="5"/>
@@ -1201,9 +1231,9 @@
       <c r="J21" s="5"/>
     </row>
     <row r="22" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>26</v>
@@ -1212,7 +1242,7 @@
         <v>23</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="5"/>
@@ -1220,9 +1250,9 @@
       <c r="J22" s="5"/>
     </row>
     <row r="23" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>26</v>
@@ -1231,7 +1261,7 @@
         <v>24</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="5"/>
@@ -1239,18 +1269,18 @@
       <c r="J23" s="5"/>
     </row>
     <row r="24" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
+      <c r="A24" s="13"/>
       <c r="B24" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="5"/>
@@ -1258,18 +1288,18 @@
       <c r="J24" s="5"/>
     </row>
     <row r="25" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
+      <c r="A25" s="13"/>
       <c r="B25" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="5"/>
@@ -1277,18 +1307,18 @@
       <c r="J25" s="5"/>
     </row>
     <row r="26" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
+      <c r="A26" s="13"/>
       <c r="B26" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="5"/>
@@ -1296,18 +1326,18 @@
       <c r="J26" s="5"/>
     </row>
     <row r="27" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
+      <c r="A27" s="13"/>
       <c r="B27" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="5"/>
@@ -1315,18 +1345,18 @@
       <c r="J27" s="5"/>
     </row>
     <row r="28" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
+      <c r="A28" s="13"/>
       <c r="B28" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
@@ -1335,7 +1365,7 @@
     </row>
     <row r="29" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>14</v>
@@ -1345,10 +1375,10 @@
         <v>15</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
@@ -1364,6 +1394,7 @@
     <mergeCell ref="A5:A8"/>
     <mergeCell ref="A10:A11"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update RTM and design of pages of Design docx
</commit_message>
<xml_diff>
--- a/Requirements/RTM.xlsx
+++ b/Requirements/RTM.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$32</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="85">
   <si>
     <t>SRS</t>
   </si>
@@ -167,14 +170,6 @@
     <t>Low_Design_transferMoney_Client_2</t>
   </si>
   <si>
-    <t>Low_Design_transferMoney_Client_1,
-Low_Design_transferMoney_Client_2</t>
-  </si>
-  <si>
-    <t>Low_Design_closeAccount_Admin_1,
-Low_Design_closeAccount_Admin_2</t>
-  </si>
-  <si>
     <t>Low_Design_closeAccount_Admin_2</t>
   </si>
   <si>
@@ -388,18 +383,7 @@
     </r>
   </si>
   <si>
-    <t>Low_Design_ViewTransaction_1</t>
-  </si>
-  <si>
-    <t>Low_Design_Display_ClientName_Date_1</t>
-  </si>
-  <si>
     <t>Low_Design_closeAccount_Admin_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Low_Design_login_1
-</t>
   </si>
   <si>
     <t>Low_Design_login_admin_2,
@@ -407,6 +391,89 @@
   </si>
   <si>
     <t xml:space="preserve">View Account </t>
+  </si>
+  <si>
+    <t>Low_Design_transferMoney_Client_1</t>
+  </si>
+  <si>
+    <t>Low_Design_Logout_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Low_Design_login_1,
+Low_Design_loginMain_1
+</t>
+  </si>
+  <si>
+    <t>Low_Design_reg_1,
+Low_Design_regMain_3</t>
+  </si>
+  <si>
+    <r>
+      <t>SRS_</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>View Account</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_003</t>
+    </r>
+  </si>
+  <si>
+    <t>CRs_2.3, CRs_4.2</t>
+  </si>
+  <si>
+    <t>Low_Design_Display_ClientName_Date_1,
+Low_Design_ViewClientMain_1</t>
+  </si>
+  <si>
+    <t>Low_Design_closeAccount_Admin_1,
+Low_Design_ViewAdminMain_1</t>
+  </si>
+  <si>
+    <t>Low_Design_transferMoney_Client_1,
+Low_Design_ViewClientMain_1</t>
+  </si>
+  <si>
+    <t>Low_Design_ViewAccountsList_Client_1</t>
+  </si>
+  <si>
+    <t>Low_Design_ViewTransaction_1,
+Low_Design_getBalance_Client_1</t>
   </si>
 </sst>
 </file>
@@ -580,7 +647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -609,6 +676,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -618,19 +688,19 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -937,26 +1007,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23:A30"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="59.42578125" defaultRowHeight="51.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54" style="2" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="36.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="39" style="2" customWidth="1"/>
-    <col min="4" max="4" width="38.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="2" customWidth="1"/>
     <col min="5" max="6" width="59.42578125" style="4"/>
     <col min="7" max="16384" width="59.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>12</v>
@@ -974,12 +1044,12 @@
         <v>1</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>34</v>
@@ -991,11 +1061,11 @@
         <v>3</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="F2" s="4"/>
-      <c r="G2" s="10" t="s">
-        <v>63</v>
+      <c r="G2" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -1012,11 +1082,13 @@
       <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="8" t="s">
+        <v>66</v>
+      </c>
       <c r="F3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="11"/>
+      <c r="G3" s="12"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -1033,17 +1105,17 @@
         <v>6</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F4" s="4"/>
-      <c r="G4" s="11"/>
+      <c r="G4" s="12"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" s="1" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>57</v>
+      <c r="A5" s="17" t="s">
+        <v>55</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>14</v>
@@ -1058,15 +1130,15 @@
         <v>76</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="G5" s="11" t="s">
-        <v>62</v>
+      <c r="G5" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="4" t="s">
         <v>28</v>
       </c>
@@ -1077,18 +1149,18 @@
         <v>11</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G6" s="11"/>
+        <v>53</v>
+      </c>
+      <c r="G6" s="12"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
@@ -1102,13 +1174,13 @@
         <v>47</v>
       </c>
       <c r="F7" s="4"/>
-      <c r="G7" s="11"/>
+      <c r="G7" s="12"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="8" t="s">
         <v>14</v>
       </c>
@@ -1122,13 +1194,13 @@
         <v>46</v>
       </c>
       <c r="F8" s="8"/>
-      <c r="G8" s="11"/>
+      <c r="G8" s="12"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="8" t="s">
         <v>14</v>
       </c>
@@ -1142,14 +1214,14 @@
         <v>46</v>
       </c>
       <c r="F9" s="8"/>
-      <c r="G9" s="11"/>
+      <c r="G9" s="12"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" s="1" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>78</v>
+      <c r="A10" s="16" t="s">
+        <v>73</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>30</v>
@@ -1158,7 +1230,7 @@
         <v>26</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>48</v>
@@ -1170,7 +1242,7 @@
       <c r="J10" s="9"/>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="8" t="s">
         <v>31</v>
       </c>
@@ -1178,10 +1250,10 @@
         <v>10</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="9"/>
@@ -1190,38 +1262,38 @@
       <c r="J11" s="9"/>
     </row>
     <row r="12" spans="1:10" s="1" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="8" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F12" s="8"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" s="1" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="9"/>
@@ -1229,39 +1301,39 @@
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
     </row>
-    <row r="14" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>58</v>
-      </c>
+    <row r="14" spans="1:10" s="1" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
       <c r="B14" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="8"/>
+        <v>30</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="D14" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>17</v>
-      </c>
       <c r="E15" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="4"/>
@@ -1270,16 +1342,18 @@
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" s="8"/>
+        <v>64</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="D16" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="4"/>
@@ -1288,16 +1362,16 @@
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="4"/>
@@ -1306,13 +1380,13 @@
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>49</v>
@@ -1324,13 +1398,13 @@
       <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>49</v>
@@ -1342,13 +1416,13 @@
       <c r="J19" s="5"/>
     </row>
     <row r="20" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>49</v>
@@ -1360,13 +1434,13 @@
       <c r="J20" s="5"/>
     </row>
     <row r="21" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>49</v>
@@ -1378,20 +1452,16 @@
       <c r="J21" s="5"/>
     </row>
     <row r="22" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>59</v>
-      </c>
+      <c r="A22" s="18"/>
       <c r="B22" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>9</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="C22" s="8"/>
       <c r="D22" s="8" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="4"/>
@@ -1400,20 +1470,20 @@
       <c r="J22" s="5"/>
     </row>
     <row r="23" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
-        <v>60</v>
+      <c r="A23" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="4"/>
@@ -1422,16 +1492,20 @@
       <c r="J23" s="5"/>
     </row>
     <row r="24" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
+      <c r="A24" s="13" t="s">
+        <v>58</v>
+      </c>
       <c r="B24" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="8"/>
+      <c r="C24" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="D24" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="4"/>
@@ -1440,16 +1514,16 @@
       <c r="J24" s="5"/>
     </row>
     <row r="25" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
+      <c r="A25" s="13"/>
       <c r="B25" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="4"/>
@@ -1458,16 +1532,16 @@
       <c r="J25" s="5"/>
     </row>
     <row r="26" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
+      <c r="A26" s="13"/>
       <c r="B26" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="4"/>
@@ -1476,18 +1550,16 @@
       <c r="J26" s="5"/>
     </row>
     <row r="27" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
+      <c r="A27" s="13"/>
       <c r="B27" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>26</v>
-      </c>
+      <c r="C27" s="8"/>
       <c r="D27" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="4"/>
@@ -1496,16 +1568,18 @@
       <c r="J27" s="5"/>
     </row>
     <row r="28" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
+      <c r="A28" s="13"/>
       <c r="B28" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="8"/>
+      <c r="C28" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="D28" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="F28" s="8"/>
       <c r="G28" s="4"/>
@@ -1514,16 +1588,16 @@
       <c r="J28" s="5"/>
     </row>
     <row r="29" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
+      <c r="A29" s="13"/>
       <c r="B29" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="4"/>
@@ -1532,54 +1606,75 @@
       <c r="J29" s="5"/>
     </row>
     <row r="30" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
+      <c r="A30" s="13"/>
       <c r="B30" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F30" s="8"/>
-      <c r="G30" s="5"/>
+      <c r="G30" s="4"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
     </row>
     <row r="31" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
-        <v>44</v>
-      </c>
+      <c r="A31" s="13"/>
       <c r="B31" s="8" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>64</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" s="8"/>
+      <c r="G31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
     </row>
+    <row r="32" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:J32"/>
   <mergeCells count="7">
     <mergeCell ref="G2:G4"/>
     <mergeCell ref="G5:G9"/>
-    <mergeCell ref="A23:A30"/>
+    <mergeCell ref="A24:A31"/>
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A10:A14"/>
     <mergeCell ref="A5:A9"/>
-    <mergeCell ref="A14:A21"/>
+    <mergeCell ref="A15:A22"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update only new high level function for reg, login and logout as omar said
</commit_message>
<xml_diff>
--- a/Requirements/RTM.xlsx
+++ b/Requirements/RTM.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B4467B-DC19-4B25-A95F-3791BF6E89F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="86">
   <si>
     <t>SRS</t>
   </si>
@@ -155,9 +154,6 @@
     <t>Logout</t>
   </si>
   <si>
-    <t>High_level_reg_1</t>
-  </si>
-  <si>
     <t>Low_Design_ViewAllAccounts_Admin_1</t>
   </si>
   <si>
@@ -167,17 +163,9 @@
     <t>Low_Design_closeAccount_Admin_2</t>
   </si>
   <si>
-    <t>High_level_Logout_admin_1,
-High_level_Logout_client_1</t>
-  </si>
-  <si>
     <t>Low_Design_addAccount_client_1</t>
   </si>
   <si>
-    <t>High_level_login_client_1,
-High_level_login_admin_1</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Register</t>
   </si>
   <si>
@@ -378,9 +366,6 @@
   </si>
   <si>
     <t>Low_Design_transferMoney_Client_1</t>
-  </si>
-  <si>
-    <t>Low_Design_Logout_1</t>
   </si>
   <si>
     <r>
@@ -441,9 +426,6 @@
   <si>
     <t xml:space="preserve">
 Low_Design_regMain_3</t>
-  </si>
-  <si>
-    <t>Low_Design_reg_1, Low_Design_reg_2</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -452,51 +434,59 @@
   </si>
   <si>
     <t>Low_Design_login_1,
-Low_Design_login_admin_2,
-Low_Design_login_client_3,
+Low_Design_login_client_2, 
+Low_Design_login_admin_1</t>
+  </si>
+  <si>
+    <t>Low_Design_login_client_2,
+Low_Design_login_admin_1</t>
+  </si>
+  <si>
+    <t>classDiagram_viewAccount_Admin_001</t>
+  </si>
+  <si>
+    <t>view_client_accounts,
+View_trans_001</t>
+  </si>
+  <si>
+    <t>classDiagram_viewAccount_Client_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Low_Design_ViewClientMain_1,
+Low_Design_transferMoney_Client_2</t>
+  </si>
+  <si>
+    <t>Low_Design_transferMoney_Client_2,
+Low_Design_ViewClientMain_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Low_Design_ViewAdminMain_1</t>
+  </si>
+  <si>
+    <t>Low_Design_closeAccount_Admin_1,
+Low_Design_closeAccount_Admin_2</t>
+  </si>
+  <si>
+    <t>High_Design_navigate_to_view_account_page_1,
+High_Design_navigate_to_admin_page_1</t>
+  </si>
+  <si>
+    <t>High_level_navigate_after_register_1</t>
+  </si>
+  <si>
+    <t>Low_Design_login_1,
 Low_Design_login_admin_1,
 Low_Design_login_client_2</t>
   </si>
   <si>
-    <t>Low_Design_login_1,
-Low_Design_login_client_2, 
-Low_Design_login_admin_1</t>
-  </si>
-  <si>
-    <t>Low_Design_login_client_2,
-Low_Design_login_admin_1</t>
-  </si>
-  <si>
-    <t>classDiagram_viewAccount_Admin_001</t>
-  </si>
-  <si>
-    <t>view_client_accounts,
-View_trans_001</t>
-  </si>
-  <si>
-    <t>classDiagram_viewAccount_Client_001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Low_Design_ViewClientMain_1,
-Low_Design_transferMoney_Client_2</t>
-  </si>
-  <si>
-    <t>Low_Design_transferMoney_Client_2,
-Low_Design_ViewClientMain_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Low_Design_ViewAdminMain_1</t>
-  </si>
-  <si>
-    <t>Low_Design_closeAccount_Admin_1,
-Low_Design_closeAccount_Admin_2</t>
+    <t>High_Design_Logout_1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -816,23 +806,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -868,23 +841,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1060,12 +1016,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="59.42578125" defaultRowHeight="51.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1080,7 +1036,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>12</v>
@@ -1098,12 +1054,12 @@
         <v>1</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>34</v>
@@ -1115,11 +1071,11 @@
         <v>3</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -1137,10 +1093,10 @@
         <v>5</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="G3" s="13"/>
       <c r="H3" s="4"/>
@@ -1157,7 +1113,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="13"/>
@@ -1167,7 +1123,7 @@
     </row>
     <row r="5" spans="1:10" s="1" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>14</v>
@@ -1179,11 +1135,11 @@
         <v>7</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -1199,10 +1155,10 @@
         <v>11</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="4"/>
@@ -1219,7 +1175,7 @@
         <v>29</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="13"/>
@@ -1237,7 +1193,7 @@
         <v>13</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="13"/>
@@ -1255,7 +1211,7 @@
         <v>35</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="13"/>
@@ -1265,7 +1221,7 @@
     </row>
     <row r="10" spans="1:10" s="1" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>30</v>
@@ -1274,14 +1230,14 @@
         <v>26</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="9" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
@@ -1293,17 +1249,17 @@
         <v>31</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="13" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
@@ -1318,10 +1274,10 @@
         <v>10</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="13"/>
@@ -1335,13 +1291,13 @@
         <v>31</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="13"/>
@@ -1358,14 +1314,14 @@
         <v>26</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="9" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
@@ -1373,21 +1329,21 @@
     </row>
     <row r="15" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8" t="s">
         <v>16</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="13" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
@@ -1396,7 +1352,7 @@
     <row r="16" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
       <c r="B16" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>25</v>
@@ -1405,7 +1361,7 @@
         <v>17</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="13"/>
@@ -1416,14 +1372,14 @@
     <row r="17" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
       <c r="B17" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8" t="s">
         <v>18</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="13"/>
@@ -1434,14 +1390,14 @@
     <row r="18" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8" t="s">
         <v>19</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="13"/>
@@ -1452,14 +1408,14 @@
     <row r="19" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
       <c r="B19" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8" t="s">
         <v>20</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="13"/>
@@ -1470,14 +1426,14 @@
     <row r="20" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
       <c r="B20" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="13"/>
@@ -1488,14 +1444,14 @@
     <row r="21" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
       <c r="B21" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8" t="s">
         <v>37</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="13"/>
@@ -1506,14 +1462,14 @@
     <row r="22" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
       <c r="B22" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8" t="s">
         <v>38</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="13"/>
@@ -1523,7 +1479,7 @@
     </row>
     <row r="23" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>32</v>
@@ -1535,7 +1491,7 @@
         <v>21</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="13"/>
@@ -1545,7 +1501,7 @@
     </row>
     <row r="24" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>30</v>
@@ -1557,11 +1513,11 @@
         <v>22</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="13" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
@@ -1577,7 +1533,7 @@
         <v>23</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="13"/>
@@ -1595,7 +1551,7 @@
         <v>24</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="13"/>
@@ -1613,7 +1569,7 @@
         <v>39</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="13"/>
@@ -1633,7 +1589,7 @@
         <v>40</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F28" s="8"/>
       <c r="G28" s="13"/>
@@ -1651,7 +1607,7 @@
         <v>41</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="13"/>
@@ -1669,7 +1625,7 @@
         <v>42</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F30" s="8"/>
       <c r="G30" s="13"/>
@@ -1687,7 +1643,7 @@
         <v>43</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F31" s="8"/>
       <c r="G31" s="13"/>
@@ -1706,21 +1662,22 @@
       <c r="D32" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E32" s="8" t="s">
-        <v>70</v>
-      </c>
+      <c r="E32" s="8"/>
       <c r="F32" s="8" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
     </row>
+    <row r="33" spans="6:6" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F33" s="8"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J32" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:J32"/>
   <mergeCells count="10">
     <mergeCell ref="G2:G4"/>
     <mergeCell ref="G5:G9"/>

</xml_diff>

<commit_message>
add perform transaction and close acount test cases IDs in RTM
</commit_message>
<xml_diff>
--- a/Requirements/RTM.xlsx
+++ b/Requirements/RTM.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="116">
   <si>
     <t>SRS</t>
   </si>
@@ -520,6 +520,28 @@
 TC_PerformTransaction_12
 TC_PerformTransaction_13
 </t>
+  </si>
+  <si>
+    <t>TC_CloseAccount_01</t>
+  </si>
+  <si>
+    <t>TC_CloseAccount_02</t>
+  </si>
+  <si>
+    <t>TC_CloseAccount_03</t>
+  </si>
+  <si>
+    <t>TC_CloseAccount_04</t>
+  </si>
+  <si>
+    <t>TC_CloseAccount_05</t>
+  </si>
+  <si>
+    <t>TC_CloseAccount_06</t>
+  </si>
+  <si>
+    <t>TC_CloseAccount_07
+TC_CloseAccount_08</t>
   </si>
 </sst>
 </file>
@@ -739,37 +761,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1079,8 +1101,8 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="59.42578125" defaultRowHeight="51.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1134,7 +1156,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="18" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1151,22 +1173,22 @@
         <v>66</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="15" t="s">
         <v>55</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="15" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="4" t="s">
         <v>33</v>
       </c>
@@ -1183,16 +1205,16 @@
       <c r="G3" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="H3" s="13"/>
+      <c r="H3" s="16"/>
       <c r="I3" s="4" t="s">
         <v>87</v>
       </c>
       <c r="J3" s="4"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="4" t="s">
         <v>32</v>
       </c>
@@ -1205,14 +1227,14 @@
         <v>59</v>
       </c>
       <c r="G4" s="4"/>
-      <c r="H4" s="13"/>
+      <c r="H4" s="16"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
     </row>
     <row r="5" spans="1:13" s="1" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="21" t="s">
         <v>49</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1229,22 +1251,22 @@
         <v>67</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="16" t="s">
         <v>54</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>90</v>
       </c>
       <c r="J5" s="4"/>
-      <c r="K5" s="13" t="s">
+      <c r="K5" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="L5" s="13" t="s">
+      <c r="L5" s="16" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="1" customFormat="1" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="4" t="s">
         <v>27</v>
       </c>
@@ -1259,16 +1281,16 @@
       <c r="G6" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="H6" s="13"/>
+      <c r="H6" s="16"/>
       <c r="I6" s="4" t="s">
         <v>87</v>
       </c>
       <c r="J6" s="4"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
     </row>
     <row r="7" spans="1:13" s="1" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
@@ -1281,14 +1303,14 @@
         <v>68</v>
       </c>
       <c r="G7" s="4"/>
-      <c r="H7" s="13"/>
+      <c r="H7" s="16"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
     </row>
     <row r="8" spans="1:13" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="7" t="s">
         <v>13</v>
       </c>
@@ -1301,14 +1323,14 @@
         <v>69</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="H8" s="13"/>
+      <c r="H8" s="16"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
     </row>
     <row r="9" spans="1:13" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="7" t="s">
         <v>13</v>
       </c>
@@ -1321,14 +1343,14 @@
         <v>69</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="H9" s="13"/>
+      <c r="H9" s="16"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
     </row>
     <row r="10" spans="1:13" s="1" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="20" t="s">
         <v>64</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -1360,7 +1382,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" s="1" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="7" t="s">
         <v>30</v>
       </c>
@@ -1375,7 +1397,7 @@
         <v>88</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="16" t="s">
         <v>71</v>
       </c>
       <c r="I11" s="8" t="s">
@@ -1384,15 +1406,15 @@
       <c r="J11" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="K11" s="13" t="s">
+      <c r="K11" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="L11" s="13" t="s">
+      <c r="L11" s="16" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="1" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="7" t="s">
         <v>30</v>
       </c>
@@ -1407,16 +1429,16 @@
         <v>80</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="H12" s="13"/>
+      <c r="H12" s="16"/>
       <c r="I12" s="8" t="s">
         <v>87</v>
       </c>
       <c r="J12" s="8"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
     </row>
     <row r="13" spans="1:13" s="1" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="7" t="s">
         <v>29</v>
       </c>
@@ -1446,7 +1468,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="22" t="s">
         <v>50</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -1456,30 +1478,30 @@
       <c r="D14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="14" t="s">
         <v>103</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>72</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="16" t="s">
         <v>71</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="K14" s="13" t="s">
+      <c r="K14" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="L14" s="13" t="s">
+      <c r="L14" s="16" t="s">
         <v>99</v>
       </c>
       <c r="M14" s="12"/>
     </row>
     <row r="15" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="7" t="s">
         <v>58</v>
       </c>
@@ -1489,49 +1511,49 @@
       <c r="D15" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="14" t="s">
         <v>102</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>73</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="H15" s="13"/>
+      <c r="H15" s="16"/>
       <c r="I15" s="5"/>
       <c r="J15" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
       <c r="M15" s="12"/>
     </row>
     <row r="16" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="7" t="s">
         <v>58</v>
       </c>
       <c r="C16" s="7"/>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="23" t="s">
+      <c r="E16" s="14" t="s">
         <v>102</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>65</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="H16" s="13"/>
+      <c r="H16" s="16"/>
       <c r="I16" s="11" t="s">
         <v>87</v>
       </c>
       <c r="J16" s="5"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
       <c r="M16" s="12"/>
     </row>
     <row r="17" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
+      <c r="A17" s="22"/>
       <c r="B17" s="7" t="s">
         <v>58</v>
       </c>
@@ -1539,22 +1561,22 @@
       <c r="D17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E17" s="13" t="s">
         <v>105</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>45</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="H17" s="13"/>
+      <c r="H17" s="16"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
       <c r="M17" s="12"/>
     </row>
     <row r="18" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="7" t="s">
         <v>58</v>
       </c>
@@ -1562,22 +1584,22 @@
       <c r="D18" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="23" t="s">
+      <c r="E18" s="14" t="s">
         <v>104</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>45</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="H18" s="13"/>
+      <c r="H18" s="16"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
       <c r="M18" s="12"/>
     </row>
     <row r="19" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="7" t="s">
         <v>58</v>
       </c>
@@ -1585,22 +1607,22 @@
       <c r="D19" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="14" t="s">
         <v>106</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>45</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="H19" s="13"/>
+      <c r="H19" s="16"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
       <c r="M19" s="12"/>
     </row>
     <row r="20" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="7" t="s">
         <v>58</v>
       </c>
@@ -1608,22 +1630,22 @@
       <c r="D20" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="E20" s="13" t="s">
         <v>107</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>45</v>
       </c>
       <c r="G20" s="7"/>
-      <c r="H20" s="13"/>
+      <c r="H20" s="16"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
       <c r="M20" s="12"/>
     </row>
     <row r="21" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
+      <c r="A21" s="22"/>
       <c r="B21" s="7" t="s">
         <v>58</v>
       </c>
@@ -1631,22 +1653,22 @@
       <c r="D21" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="22" t="s">
+      <c r="E21" s="13" t="s">
         <v>108</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>45</v>
       </c>
       <c r="G21" s="7"/>
-      <c r="H21" s="13"/>
+      <c r="H21" s="16"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
       <c r="M21" s="12"/>
     </row>
     <row r="22" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="23" t="s">
         <v>51</v>
       </c>
       <c r="B22" s="7" t="s">
@@ -1663,17 +1685,17 @@
         <v>47</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="H22" s="13"/>
+      <c r="H22" s="16"/>
       <c r="I22" s="11" t="s">
         <v>87</v>
       </c>
       <c r="J22" s="5"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
       <c r="M22" s="12"/>
     </row>
     <row r="23" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
+      <c r="A23" s="23"/>
       <c r="B23" s="7" t="s">
         <v>31</v>
       </c>
@@ -1686,15 +1708,15 @@
         <v>47</v>
       </c>
       <c r="G23" s="7"/>
-      <c r="H23" s="13"/>
+      <c r="H23" s="16"/>
       <c r="I23" s="11"/>
       <c r="J23" s="5"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
       <c r="M23" s="12"/>
     </row>
     <row r="24" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="17" t="s">
         <v>52</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -1706,27 +1728,29 @@
       <c r="D24" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="7"/>
+      <c r="E24" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="F24" s="7" t="s">
         <v>74</v>
       </c>
       <c r="G24" s="7"/>
-      <c r="H24" s="13" t="s">
+      <c r="H24" s="16" t="s">
         <v>70</v>
       </c>
       <c r="I24" s="5"/>
       <c r="J24" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="K24" s="13" t="s">
+      <c r="K24" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="L24" s="13" t="s">
+      <c r="L24" s="16" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
+      <c r="A25" s="17"/>
       <c r="B25" s="7" t="s">
         <v>29</v>
       </c>
@@ -1734,19 +1758,21 @@
       <c r="D25" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="7"/>
+      <c r="E25" s="7" t="s">
+        <v>110</v>
+      </c>
       <c r="F25" s="7" t="s">
         <v>46</v>
       </c>
       <c r="G25" s="7"/>
-      <c r="H25" s="13"/>
+      <c r="H25" s="16"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
     </row>
     <row r="26" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
+      <c r="A26" s="17"/>
       <c r="B26" s="7" t="s">
         <v>29</v>
       </c>
@@ -1754,19 +1780,21 @@
       <c r="D26" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="7"/>
+      <c r="E26" s="7" t="s">
+        <v>111</v>
+      </c>
       <c r="F26" s="7" t="s">
         <v>46</v>
       </c>
       <c r="G26" s="7"/>
-      <c r="H26" s="13"/>
+      <c r="H26" s="16"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
     </row>
     <row r="27" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
+      <c r="A27" s="17"/>
       <c r="B27" s="7" t="s">
         <v>29</v>
       </c>
@@ -1774,19 +1802,21 @@
       <c r="D27" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="7"/>
+      <c r="E27" s="7" t="s">
+        <v>112</v>
+      </c>
       <c r="F27" s="7" t="s">
         <v>46</v>
       </c>
       <c r="G27" s="7"/>
-      <c r="H27" s="13"/>
+      <c r="H27" s="16"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
     </row>
     <row r="28" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
+      <c r="A28" s="17"/>
       <c r="B28" s="7" t="s">
         <v>29</v>
       </c>
@@ -1796,19 +1826,21 @@
       <c r="D28" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E28" s="7"/>
+      <c r="E28" s="7" t="s">
+        <v>113</v>
+      </c>
       <c r="F28" s="7" t="s">
         <v>46</v>
       </c>
       <c r="G28" s="7"/>
-      <c r="H28" s="13"/>
+      <c r="H28" s="16"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
     </row>
     <row r="29" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
+      <c r="A29" s="17"/>
       <c r="B29" s="7" t="s">
         <v>29</v>
       </c>
@@ -1816,21 +1848,23 @@
       <c r="D29" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E29" s="7"/>
+      <c r="E29" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="F29" s="7" t="s">
         <v>75</v>
       </c>
       <c r="G29" s="7"/>
-      <c r="H29" s="13"/>
+      <c r="H29" s="16"/>
       <c r="I29" s="10" t="s">
         <v>87</v>
       </c>
       <c r="J29" s="5"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
     </row>
     <row r="30" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
+      <c r="A30" s="17"/>
       <c r="B30" s="7" t="s">
         <v>29</v>
       </c>
@@ -1838,19 +1872,21 @@
       <c r="D30" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E30" s="7"/>
+      <c r="E30" s="7" t="s">
+        <v>114</v>
+      </c>
       <c r="F30" s="7" t="s">
         <v>46</v>
       </c>
       <c r="G30" s="7"/>
-      <c r="H30" s="13"/>
+      <c r="H30" s="16"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
     </row>
     <row r="31" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
+      <c r="A31" s="17"/>
       <c r="B31" s="7" t="s">
         <v>29</v>
       </c>
@@ -1858,16 +1894,18 @@
       <c r="D31" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E31" s="7"/>
+      <c r="E31" s="7" t="s">
+        <v>115</v>
+      </c>
       <c r="F31" s="7" t="s">
         <v>46</v>
       </c>
       <c r="G31" s="7"/>
-      <c r="H31" s="13"/>
+      <c r="H31" s="16"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
     </row>
     <row r="32" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
@@ -1905,11 +1943,6 @@
   </sheetData>
   <autoFilter ref="A1:K32"/>
   <mergeCells count="21">
-    <mergeCell ref="L2:L4"/>
-    <mergeCell ref="L5:L9"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="L14:L23"/>
-    <mergeCell ref="L24:L31"/>
     <mergeCell ref="H14:H23"/>
     <mergeCell ref="K14:K23"/>
     <mergeCell ref="H2:H4"/>
@@ -1926,6 +1959,11 @@
     <mergeCell ref="K2:K4"/>
     <mergeCell ref="K5:K9"/>
     <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="L5:L9"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L14:L23"/>
+    <mergeCell ref="L24:L31"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update for next baseline
</commit_message>
<xml_diff>
--- a/Requirements/RTM.xlsx
+++ b/Requirements/RTM.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE62BB81-55AC-4619-98C2-58374021CC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="129">
   <si>
     <t>SRS</t>
   </si>
@@ -558,23 +559,69 @@
 TC_Login_006,TC_Login_007</t>
   </si>
   <si>
+    <t>TC_Add New Account _001</t>
+  </si>
+  <si>
+    <t>TC_Add New Account _002</t>
+  </si>
+  <si>
+    <t>TC_Register_001</t>
+  </si>
+  <si>
+    <t>TC_Register_002
+TC_Register_003
+TC_Register_004
+TC_Register_005
+TC_Register_006
+TC_Register_007
+TC_Register_008
+TC_Register_009
+TC_Register_010
+TC_Register_011
+TC_Register_012
+TC_Register_013
+TC_Register_014
+TC_Register_015
+TC_Register_016
+TC_Register_017
+TC_Register_018
+TC_Register_019
+TC_Register_020
+TC_Register_021
+TC_Register_022
+TC_Register_023
+TC_Register_024</t>
+  </si>
+  <si>
+    <t>TC_ViwAccount_001
+TC_ViwAccount_003
+TC_ViwAccount_004
+TC_ViwAccount_005
+TC_ViwAccount_006</t>
+  </si>
+  <si>
+    <t>TC_ViwAccount_009
+TC_ViwAccount_011
+TC_ViwAccount_012
+TC_ViwAccount_013</t>
+  </si>
+  <si>
+    <t>TC_ViwAccount_010</t>
+  </si>
+  <si>
+    <t>TC_ViwAccount_002</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC_Logout _001_client
 TC_Logout _001_Admin
-TC_Logout _002  
 </t>
-  </si>
-  <si>
-    <t>TC_Add New Account _001</t>
-  </si>
-  <si>
-    <t>TC_Add New Account _002</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -668,13 +715,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="10">
@@ -816,15 +856,12 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -845,6 +882,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -939,6 +979,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -974,6 +1031,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1149,12 +1223,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="59.42578125" defaultRowHeight="51.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1208,7 +1282,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1220,27 +1294,29 @@
       <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="11"/>
+      <c r="E2" s="11" t="s">
+        <v>122</v>
+      </c>
       <c r="F2" s="7" t="s">
         <v>66</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="16" t="s">
         <v>55</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="L2" s="16" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="4" t="s">
         <v>33</v>
       </c>
@@ -1250,7 +1326,9 @@
       <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="11"/>
+      <c r="E3" s="11" t="s">
+        <v>122</v>
+      </c>
       <c r="F3" s="7" t="s">
         <v>59</v>
       </c>
@@ -1265,8 +1343,8 @@
       <c r="K3" s="17"/>
       <c r="L3" s="17"/>
     </row>
-    <row r="4" spans="1:13" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
+    <row r="4" spans="1:13" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
       <c r="B4" s="4" t="s">
         <v>32</v>
       </c>
@@ -1274,7 +1352,9 @@
       <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="11"/>
+      <c r="E4" s="7" t="s">
+        <v>123</v>
+      </c>
       <c r="F4" s="7" t="s">
         <v>59</v>
       </c>
@@ -1286,7 +1366,7 @@
       <c r="L4" s="17"/>
     </row>
     <row r="5" spans="1:13" s="1" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="22" t="s">
         <v>49</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1320,7 +1400,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" s="1" customFormat="1" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="4" t="s">
         <v>27</v>
       </c>
@@ -1346,7 +1426,7 @@
       <c r="L6" s="17"/>
     </row>
     <row r="7" spans="1:13" s="1" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
@@ -1368,7 +1448,7 @@
       <c r="L7" s="17"/>
     </row>
     <row r="8" spans="1:13" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="7" t="s">
         <v>13</v>
       </c>
@@ -1390,7 +1470,7 @@
       <c r="L8" s="17"/>
     </row>
     <row r="9" spans="1:13" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="7" t="s">
         <v>13</v>
       </c>
@@ -1411,8 +1491,8 @@
       <c r="K9" s="17"/>
       <c r="L9" s="17"/>
     </row>
-    <row r="10" spans="1:13" s="1" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+    <row r="10" spans="1:13" s="1" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
         <v>64</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -1424,7 +1504,9 @@
       <c r="D10" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="7" t="s">
+        <v>124</v>
+      </c>
       <c r="F10" s="7" t="s">
         <v>44</v>
       </c>
@@ -1444,7 +1526,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" s="1" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="7" t="s">
         <v>30</v>
       </c>
@@ -1454,7 +1536,9 @@
       <c r="D11" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="7"/>
+      <c r="E11" s="7" t="s">
+        <v>125</v>
+      </c>
       <c r="F11" s="7" t="s">
         <v>88</v>
       </c>
@@ -1476,7 +1560,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" s="1" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="7" t="s">
         <v>30</v>
       </c>
@@ -1486,7 +1570,9 @@
       <c r="D12" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="7"/>
+      <c r="E12" s="7" t="s">
+        <v>126</v>
+      </c>
       <c r="F12" s="7" t="s">
         <v>80</v>
       </c>
@@ -1500,7 +1586,7 @@
       <c r="L12" s="17"/>
     </row>
     <row r="13" spans="1:13" s="1" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="7" t="s">
         <v>29</v>
       </c>
@@ -1510,7 +1596,9 @@
       <c r="D13" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="7"/>
+      <c r="E13" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="F13" s="7" t="s">
         <v>44</v>
       </c>
@@ -1530,7 +1618,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="23" t="s">
         <v>50</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -1563,7 +1651,7 @@
       <c r="M14" s="12"/>
     </row>
     <row r="15" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="7" t="s">
         <v>58</v>
       </c>
@@ -1590,7 +1678,7 @@
       <c r="M15" s="12"/>
     </row>
     <row r="16" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="7" t="s">
         <v>58</v>
       </c>
@@ -1615,7 +1703,7 @@
       <c r="M16" s="12"/>
     </row>
     <row r="17" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="7" t="s">
         <v>58</v>
       </c>
@@ -1638,7 +1726,7 @@
       <c r="M17" s="12"/>
     </row>
     <row r="18" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="7" t="s">
         <v>58</v>
       </c>
@@ -1661,7 +1749,7 @@
       <c r="M18" s="12"/>
     </row>
     <row r="19" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="7" t="s">
         <v>58</v>
       </c>
@@ -1684,7 +1772,7 @@
       <c r="M19" s="12"/>
     </row>
     <row r="20" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="7" t="s">
         <v>58</v>
       </c>
@@ -1707,7 +1795,7 @@
       <c r="M20" s="12"/>
     </row>
     <row r="21" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="7" t="s">
         <v>58</v>
       </c>
@@ -1730,7 +1818,7 @@
       <c r="M21" s="12"/>
     </row>
     <row r="22" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="24" t="s">
         <v>51</v>
       </c>
       <c r="B22" s="7" t="s">
@@ -1743,7 +1831,7 @@
         <v>20</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>47</v>
@@ -1759,7 +1847,7 @@
       <c r="M22" s="12"/>
     </row>
     <row r="23" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
+      <c r="A23" s="24"/>
       <c r="B23" s="7" t="s">
         <v>31</v>
       </c>
@@ -1768,7 +1856,7 @@
         <v>81</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>47</v>
@@ -1782,7 +1870,7 @@
       <c r="M23" s="12"/>
     </row>
     <row r="24" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="18" t="s">
         <v>52</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -1816,7 +1904,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
+      <c r="A25" s="18"/>
       <c r="B25" s="7" t="s">
         <v>29</v>
       </c>
@@ -1838,7 +1926,7 @@
       <c r="L25" s="17"/>
     </row>
     <row r="26" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
+      <c r="A26" s="18"/>
       <c r="B26" s="7" t="s">
         <v>29</v>
       </c>
@@ -1860,7 +1948,7 @@
       <c r="L26" s="17"/>
     </row>
     <row r="27" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="19"/>
+      <c r="A27" s="18"/>
       <c r="B27" s="7" t="s">
         <v>29</v>
       </c>
@@ -1882,7 +1970,7 @@
       <c r="L27" s="17"/>
     </row>
     <row r="28" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
+      <c r="A28" s="18"/>
       <c r="B28" s="7" t="s">
         <v>29</v>
       </c>
@@ -1906,7 +1994,7 @@
       <c r="L28" s="17"/>
     </row>
     <row r="29" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
+      <c r="A29" s="18"/>
       <c r="B29" s="7" t="s">
         <v>29</v>
       </c>
@@ -1930,7 +2018,7 @@
       <c r="L29" s="17"/>
     </row>
     <row r="30" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
+      <c r="A30" s="18"/>
       <c r="B30" s="7" t="s">
         <v>29</v>
       </c>
@@ -1952,7 +2040,7 @@
       <c r="L30" s="17"/>
     </row>
     <row r="31" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
+      <c r="A31" s="18"/>
       <c r="B31" s="7" t="s">
         <v>29</v>
       </c>
@@ -1984,8 +2072,8 @@
       <c r="D32" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="16" t="s">
-        <v>120</v>
+      <c r="E32" s="25" t="s">
+        <v>128</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="7" t="s">
@@ -2009,13 +2097,8 @@
       <c r="G33" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K32"/>
+  <autoFilter ref="A1:K32" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="21">
-    <mergeCell ref="L2:L4"/>
-    <mergeCell ref="L5:L9"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="L14:L23"/>
-    <mergeCell ref="L24:L31"/>
     <mergeCell ref="H14:H23"/>
     <mergeCell ref="K14:K23"/>
     <mergeCell ref="H2:H4"/>
@@ -2032,6 +2115,11 @@
     <mergeCell ref="K2:K4"/>
     <mergeCell ref="K5:K9"/>
     <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="L5:L9"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L14:L23"/>
+    <mergeCell ref="L24:L31"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update as per reviews
</commit_message>
<xml_diff>
--- a/Requirements/RTM.xlsx
+++ b/Requirements/RTM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE62BB81-55AC-4619-98C2-58374021CC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4EE17E-E9A5-4BE1-9F18-075041C337A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,14 +11,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$35</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="132">
   <si>
     <t>SRS</t>
   </si>
@@ -615,6 +615,15 @@
     <t xml:space="preserve">TC_Logout _001_client
 TC_Logout _001_Admin
 </t>
+  </si>
+  <si>
+    <t>SRS_PerformTransaction_009</t>
+  </si>
+  <si>
+    <t>SRS_PerformTransaction_010</t>
+  </si>
+  <si>
+    <t>SRS_PerformTransaction_011</t>
   </si>
 </sst>
 </file>
@@ -809,7 +818,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -856,12 +865,18 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -882,9 +897,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1224,11 +1236,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="59.42578125" defaultRowHeight="51.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1282,7 +1294,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="21" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1301,22 +1313,22 @@
         <v>66</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="19" t="s">
         <v>55</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="L2" s="19" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="4" t="s">
         <v>33</v>
       </c>
@@ -1335,16 +1347,16 @@
       <c r="G3" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="H3" s="17"/>
+      <c r="H3" s="18"/>
       <c r="I3" s="4" t="s">
         <v>87</v>
       </c>
       <c r="J3" s="4"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="4" t="s">
         <v>32</v>
       </c>
@@ -1359,14 +1371,14 @@
         <v>59</v>
       </c>
       <c r="G4" s="4"/>
-      <c r="H4" s="17"/>
+      <c r="H4" s="18"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
     </row>
     <row r="5" spans="1:13" s="1" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="24" t="s">
         <v>49</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1385,22 +1397,22 @@
         <v>67</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="18" t="s">
         <v>54</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>90</v>
       </c>
       <c r="J5" s="4"/>
-      <c r="K5" s="17" t="s">
+      <c r="K5" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="L5" s="18" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="1" customFormat="1" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="4" t="s">
         <v>27</v>
       </c>
@@ -1417,16 +1429,16 @@
       <c r="G6" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="H6" s="17"/>
+      <c r="H6" s="18"/>
       <c r="I6" s="4" t="s">
         <v>87</v>
       </c>
       <c r="J6" s="4"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
     </row>
     <row r="7" spans="1:13" s="1" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
@@ -1441,14 +1453,14 @@
         <v>68</v>
       </c>
       <c r="G7" s="4"/>
-      <c r="H7" s="17"/>
+      <c r="H7" s="18"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
     </row>
     <row r="8" spans="1:13" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="7" t="s">
         <v>13</v>
       </c>
@@ -1463,14 +1475,14 @@
         <v>69</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="H8" s="17"/>
+      <c r="H8" s="18"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
     </row>
     <row r="9" spans="1:13" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="7" t="s">
         <v>13</v>
       </c>
@@ -1485,14 +1497,14 @@
         <v>69</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="H9" s="17"/>
+      <c r="H9" s="18"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
     </row>
     <row r="10" spans="1:13" s="1" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="23" t="s">
         <v>64</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -1526,7 +1538,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" s="1" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="7" t="s">
         <v>30</v>
       </c>
@@ -1543,7 +1555,7 @@
         <v>88</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="18" t="s">
         <v>71</v>
       </c>
       <c r="I11" s="8" t="s">
@@ -1552,15 +1564,15 @@
       <c r="J11" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="K11" s="17" t="s">
+      <c r="K11" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="L11" s="17" t="s">
+      <c r="L11" s="18" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="1" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="7" t="s">
         <v>30</v>
       </c>
@@ -1577,16 +1589,16 @@
         <v>80</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="H12" s="17"/>
+      <c r="H12" s="18"/>
       <c r="I12" s="8" t="s">
         <v>87</v>
       </c>
       <c r="J12" s="8"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
     </row>
     <row r="13" spans="1:13" s="1" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="7" t="s">
         <v>29</v>
       </c>
@@ -1618,7 +1630,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="25" t="s">
         <v>50</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -1635,23 +1647,23 @@
         <v>72</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="H14" s="17" t="s">
+      <c r="H14" s="18" t="s">
         <v>71</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="K14" s="17" t="s">
+      <c r="K14" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="L14" s="17" t="s">
+      <c r="L14" s="18" t="s">
         <v>99</v>
       </c>
       <c r="M14" s="12"/>
     </row>
     <row r="15" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="7" t="s">
         <v>58</v>
       </c>
@@ -1668,17 +1680,17 @@
         <v>73</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="H15" s="17"/>
+      <c r="H15" s="18"/>
       <c r="I15" s="5"/>
       <c r="J15" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
       <c r="M15" s="12"/>
     </row>
     <row r="16" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="7" t="s">
         <v>58</v>
       </c>
@@ -1693,17 +1705,17 @@
         <v>65</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="H16" s="17"/>
+      <c r="H16" s="18"/>
       <c r="I16" s="11" t="s">
         <v>87</v>
       </c>
       <c r="J16" s="5"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
       <c r="M16" s="12"/>
     </row>
     <row r="17" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="7" t="s">
         <v>58</v>
       </c>
@@ -1718,15 +1730,15 @@
         <v>45</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="H17" s="17"/>
+      <c r="H17" s="18"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
       <c r="M17" s="12"/>
     </row>
     <row r="18" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="7" t="s">
         <v>58</v>
       </c>
@@ -1741,15 +1753,15 @@
         <v>45</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="H18" s="17"/>
+      <c r="H18" s="18"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
       <c r="M18" s="12"/>
     </row>
     <row r="19" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="7" t="s">
         <v>58</v>
       </c>
@@ -1764,15 +1776,15 @@
         <v>45</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="H19" s="17"/>
+      <c r="H19" s="18"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
       <c r="M19" s="12"/>
     </row>
     <row r="20" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="7" t="s">
         <v>58</v>
       </c>
@@ -1787,15 +1799,15 @@
         <v>45</v>
       </c>
       <c r="G20" s="7"/>
-      <c r="H20" s="17"/>
+      <c r="H20" s="18"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
+    <row r="21" spans="1:13" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="25"/>
       <c r="B21" s="7" t="s">
         <v>58</v>
       </c>
@@ -1810,316 +1822,379 @@
         <v>45</v>
       </c>
       <c r="G21" s="7"/>
-      <c r="H21" s="17"/>
+      <c r="H21" s="18"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
-        <v>51</v>
-      </c>
+    <row r="22" spans="1:13" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
       <c r="B22" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>9</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="C22" s="7"/>
       <c r="D22" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>120</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="E22" s="13"/>
       <c r="F22" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="11" t="s">
-        <v>87</v>
-      </c>
+      <c r="H22" s="18"/>
+      <c r="I22" s="5"/>
       <c r="J22" s="5"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="24"/>
+    <row r="23" spans="1:13" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="16"/>
       <c r="B23" s="7" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>121</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="E23" s="13"/>
       <c r="F23" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23" s="7"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="12"/>
+    </row>
+    <row r="24" spans="1:13" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16"/>
+      <c r="B24" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E24" s="13"/>
+      <c r="F24" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G24" s="7"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="12"/>
+    </row>
+    <row r="25" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="F25" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G23" s="7"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="12"/>
-    </row>
-    <row r="24" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G24" s="7"/>
-      <c r="H24" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="I24" s="5"/>
-      <c r="J24" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="K24" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="L24" s="17" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
-      <c r="B25" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>46</v>
-      </c>
       <c r="G25" s="7"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="5"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="11" t="s">
+        <v>87</v>
+      </c>
       <c r="J25" s="5"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="12"/>
     </row>
     <row r="26" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
+      <c r="A26" s="26"/>
       <c r="B26" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7" t="s">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G26" s="7"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="5"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="11"/>
       <c r="J26" s="5"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="12"/>
     </row>
     <row r="27" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
+      <c r="A27" s="20" t="s">
+        <v>52</v>
+      </c>
       <c r="B27" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="7"/>
+      <c r="C27" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="D27" s="7" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="G27" s="7"/>
-      <c r="H27" s="17"/>
+      <c r="H27" s="18" t="s">
+        <v>70</v>
+      </c>
       <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
+      <c r="J27" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="K27" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="L27" s="18" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="28" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
+      <c r="A28" s="20"/>
       <c r="B28" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>25</v>
-      </c>
+      <c r="C28" s="7"/>
       <c r="D28" s="7" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F28" s="7" t="s">
         <v>46</v>
       </c>
       <c r="G28" s="7"/>
-      <c r="H28" s="17"/>
+      <c r="H28" s="18"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
     </row>
     <row r="29" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
+      <c r="A29" s="20"/>
       <c r="B29" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="G29" s="7"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="10" t="s">
-        <v>87</v>
-      </c>
+      <c r="H29" s="18"/>
+      <c r="I29" s="5"/>
       <c r="J29" s="5"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
     </row>
     <row r="30" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
+      <c r="A30" s="20"/>
       <c r="B30" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F30" s="7" t="s">
         <v>46</v>
       </c>
       <c r="G30" s="7"/>
-      <c r="H30" s="17"/>
+      <c r="H30" s="18"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
     </row>
     <row r="31" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
+      <c r="A31" s="20"/>
       <c r="B31" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="7"/>
+      <c r="C31" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="D31" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>46</v>
       </c>
       <c r="G31" s="7"/>
-      <c r="H31" s="17"/>
+      <c r="H31" s="18"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
-      <c r="K31" s="17"/>
-      <c r="L31" s="17"/>
-    </row>
-    <row r="32" spans="1:13" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>43</v>
-      </c>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+    </row>
+    <row r="32" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="20"/>
       <c r="B32" s="7" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G32" s="7"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="J32" s="5"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+    </row>
+    <row r="33" spans="1:12" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="20"/>
+      <c r="B33" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G33" s="7"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+    </row>
+    <row r="34" spans="1:12" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="20"/>
+      <c r="B34" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G34" s="7"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
+    </row>
+    <row r="35" spans="1:12" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="25" t="s">
+      <c r="E35" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7" t="s">
+      <c r="F35" s="7"/>
+      <c r="G35" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="H32" s="7" t="s">
+      <c r="H35" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="I32" s="5"/>
-      <c r="J32" s="10" t="s">
+      <c r="I35" s="5"/>
+      <c r="J35" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="K32" s="10" t="s">
+      <c r="K35" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="L32" s="7" t="s">
+      <c r="L35" s="7" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="7:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G33" s="7"/>
+    <row r="36" spans="1:12" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G36" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K32" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:K35" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="21">
-    <mergeCell ref="H14:H23"/>
-    <mergeCell ref="K14:K23"/>
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="L5:L9"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L14:L26"/>
+    <mergeCell ref="L27:L34"/>
+    <mergeCell ref="H14:H26"/>
+    <mergeCell ref="K14:K26"/>
     <mergeCell ref="H2:H4"/>
     <mergeCell ref="H5:H9"/>
-    <mergeCell ref="A24:A31"/>
+    <mergeCell ref="A27:A34"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="A5:A9"/>
     <mergeCell ref="A14:A21"/>
     <mergeCell ref="H11:H12"/>
-    <mergeCell ref="H24:H31"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="K24:K31"/>
+    <mergeCell ref="H27:H34"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="K27:K34"/>
     <mergeCell ref="K2:K4"/>
     <mergeCell ref="K5:K9"/>
     <mergeCell ref="K11:K12"/>
-    <mergeCell ref="L2:L4"/>
-    <mergeCell ref="L5:L9"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="L14:L23"/>
-    <mergeCell ref="L24:L31"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update perform transaction test cases
</commit_message>
<xml_diff>
--- a/Requirements/RTM.xlsx
+++ b/Requirements/RTM.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4EE17E-E9A5-4BE1-9F18-075041C337A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="135">
   <si>
     <t>SRS</t>
   </si>
@@ -504,11 +503,6 @@
     <t>TC_PerformTransaction_03</t>
   </si>
   <si>
-    <t>TC_PerformTransaction_02
-TC_PerformTransaction_05
-TC_PerformTransaction_06</t>
-  </si>
-  <si>
     <t>TC_PerformTransaction_07</t>
   </si>
   <si>
@@ -625,11 +619,24 @@
   <si>
     <t>SRS_PerformTransaction_011</t>
   </si>
+  <si>
+    <t>TC_PerformTransaction_02
+TC_PerformTransaction_06</t>
+  </si>
+  <si>
+    <t>TC_PerformTransaction_05</t>
+  </si>
+  <si>
+    <t>TC_PerformTransaction_14</t>
+  </si>
+  <si>
+    <t>TC_PerformTransaction_15</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -871,10 +878,10 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -991,23 +998,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1043,23 +1033,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1235,12 +1208,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="59.42578125" defaultRowHeight="51.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1307,23 +1280,23 @@
         <v>3</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>66</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="18" t="s">
         <v>55</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="L2" s="19" t="s">
+      <c r="L2" s="18" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1339,7 +1312,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>59</v>
@@ -1347,13 +1320,13 @@
       <c r="G3" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="H3" s="18"/>
+      <c r="H3" s="19"/>
       <c r="I3" s="4" t="s">
         <v>87</v>
       </c>
       <c r="J3" s="4"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
@@ -1365,17 +1338,17 @@
         <v>6</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>59</v>
       </c>
       <c r="G4" s="4"/>
-      <c r="H4" s="18"/>
+      <c r="H4" s="19"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
     </row>
     <row r="5" spans="1:13" s="1" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
@@ -1391,23 +1364,23 @@
         <v>7</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>67</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="19" t="s">
         <v>54</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>90</v>
       </c>
       <c r="J5" s="4"/>
-      <c r="K5" s="18" t="s">
+      <c r="K5" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="L5" s="18" t="s">
+      <c r="L5" s="19" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1421,7 +1394,7 @@
         <v>10</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>78</v>
@@ -1429,13 +1402,13 @@
       <c r="G6" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="H6" s="18"/>
+      <c r="H6" s="19"/>
       <c r="I6" s="4" t="s">
         <v>87</v>
       </c>
       <c r="J6" s="4"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
     </row>
     <row r="7" spans="1:13" s="1" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24"/>
@@ -1447,17 +1420,17 @@
         <v>28</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>68</v>
       </c>
       <c r="G7" s="4"/>
-      <c r="H7" s="18"/>
+      <c r="H7" s="19"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
     </row>
     <row r="8" spans="1:13" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
@@ -1469,17 +1442,17 @@
         <v>12</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>69</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="H8" s="18"/>
+      <c r="H8" s="19"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
     </row>
     <row r="9" spans="1:13" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
@@ -1491,17 +1464,17 @@
         <v>34</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>69</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="H9" s="18"/>
+      <c r="H9" s="19"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
     </row>
     <row r="10" spans="1:13" s="1" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
@@ -1517,7 +1490,7 @@
         <v>60</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>44</v>
@@ -1549,13 +1522,13 @@
         <v>61</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>88</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="19" t="s">
         <v>71</v>
       </c>
       <c r="I11" s="8" t="s">
@@ -1564,10 +1537,10 @@
       <c r="J11" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="K11" s="18" t="s">
+      <c r="K11" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="L11" s="18" t="s">
+      <c r="L11" s="19" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1583,19 +1556,19 @@
         <v>62</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>80</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="H12" s="18"/>
+      <c r="H12" s="19"/>
       <c r="I12" s="8" t="s">
         <v>87</v>
       </c>
       <c r="J12" s="8"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
     </row>
     <row r="13" spans="1:13" s="1" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23"/>
@@ -1609,7 +1582,7 @@
         <v>63</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>44</v>
@@ -1647,17 +1620,17 @@
         <v>72</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="19" t="s">
         <v>71</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="K14" s="18" t="s">
+      <c r="K14" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="L14" s="18" t="s">
+      <c r="L14" s="19" t="s">
         <v>99</v>
       </c>
       <c r="M14" s="12"/>
@@ -1680,13 +1653,13 @@
         <v>73</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="H15" s="18"/>
+      <c r="H15" s="19"/>
       <c r="I15" s="5"/>
       <c r="J15" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
       <c r="M15" s="12"/>
     </row>
     <row r="16" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1705,13 +1678,13 @@
         <v>65</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="H16" s="18"/>
+      <c r="H16" s="19"/>
       <c r="I16" s="11" t="s">
         <v>87</v>
       </c>
       <c r="J16" s="5"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
       <c r="M16" s="12"/>
     </row>
     <row r="17" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1724,17 +1697,17 @@
         <v>18</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>45</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="H17" s="18"/>
+      <c r="H17" s="19"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
       <c r="M17" s="12"/>
     </row>
     <row r="18" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1753,11 +1726,11 @@
         <v>45</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="H18" s="18"/>
+      <c r="H18" s="19"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
       <c r="M18" s="12"/>
     </row>
     <row r="19" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1770,17 +1743,17 @@
         <v>35</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>45</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="H19" s="18"/>
+      <c r="H19" s="19"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
       <c r="M19" s="12"/>
     </row>
     <row r="20" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1793,17 +1766,17 @@
         <v>36</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>45</v>
       </c>
       <c r="G20" s="7"/>
-      <c r="H20" s="18"/>
+      <c r="H20" s="19"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
       <c r="M20" s="12"/>
     </row>
     <row r="21" spans="1:13" ht="84" customHeight="1" x14ac:dyDescent="0.25">
@@ -1816,17 +1789,17 @@
         <v>37</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>45</v>
       </c>
       <c r="G21" s="7"/>
-      <c r="H21" s="18"/>
+      <c r="H21" s="19"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
       <c r="M21" s="12"/>
     </row>
     <row r="22" spans="1:13" ht="84" customHeight="1" x14ac:dyDescent="0.25">
@@ -1836,18 +1809,20 @@
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="E22" s="13"/>
+        <v>128</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>132</v>
+      </c>
       <c r="F22" s="7" t="s">
         <v>45</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="H22" s="18"/>
+      <c r="H22" s="19"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
       <c r="M22" s="12"/>
     </row>
     <row r="23" spans="1:13" ht="84" customHeight="1" x14ac:dyDescent="0.25">
@@ -1857,18 +1832,20 @@
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="E23" s="13"/>
+        <v>129</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>133</v>
+      </c>
       <c r="F23" s="7" t="s">
         <v>45</v>
       </c>
       <c r="G23" s="7"/>
-      <c r="H23" s="18"/>
+      <c r="H23" s="19"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
       <c r="M23" s="12"/>
     </row>
     <row r="24" spans="1:13" ht="84" customHeight="1" x14ac:dyDescent="0.25">
@@ -1878,18 +1855,20 @@
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="E24" s="13"/>
+        <v>130</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>134</v>
+      </c>
       <c r="F24" s="7" t="s">
         <v>45</v>
       </c>
       <c r="G24" s="7"/>
-      <c r="H24" s="18"/>
+      <c r="H24" s="19"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
       <c r="M24" s="12"/>
     </row>
     <row r="25" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1906,19 +1885,19 @@
         <v>20</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>47</v>
       </c>
       <c r="G25" s="7"/>
-      <c r="H25" s="18"/>
+      <c r="H25" s="19"/>
       <c r="I25" s="11" t="s">
         <v>87</v>
       </c>
       <c r="J25" s="5"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="18"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
       <c r="M25" s="12"/>
     </row>
     <row r="26" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1931,17 +1910,17 @@
         <v>81</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>47</v>
       </c>
       <c r="G26" s="7"/>
-      <c r="H26" s="18"/>
+      <c r="H26" s="19"/>
       <c r="I26" s="11"/>
       <c r="J26" s="5"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
       <c r="M26" s="12"/>
     </row>
     <row r="27" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1958,23 +1937,23 @@
         <v>21</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>74</v>
       </c>
       <c r="G27" s="7"/>
-      <c r="H27" s="18" t="s">
+      <c r="H27" s="19" t="s">
         <v>70</v>
       </c>
       <c r="I27" s="5"/>
       <c r="J27" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="K27" s="18" t="s">
+      <c r="K27" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="L27" s="18" t="s">
+      <c r="L27" s="19" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1988,17 +1967,17 @@
         <v>22</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F28" s="7" t="s">
         <v>46</v>
       </c>
       <c r="G28" s="7"/>
-      <c r="H28" s="18"/>
+      <c r="H28" s="19"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
     </row>
     <row r="29" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20"/>
@@ -2010,17 +1989,17 @@
         <v>23</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>46</v>
       </c>
       <c r="G29" s="7"/>
-      <c r="H29" s="18"/>
+      <c r="H29" s="19"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
     </row>
     <row r="30" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="20"/>
@@ -2032,17 +2011,17 @@
         <v>38</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F30" s="7" t="s">
         <v>46</v>
       </c>
       <c r="G30" s="7"/>
-      <c r="H30" s="18"/>
+      <c r="H30" s="19"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
     </row>
     <row r="31" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20"/>
@@ -2056,17 +2035,17 @@
         <v>39</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>46</v>
       </c>
       <c r="G31" s="7"/>
-      <c r="H31" s="18"/>
+      <c r="H31" s="19"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="18"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
     </row>
     <row r="32" spans="1:13" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="20"/>
@@ -2078,19 +2057,19 @@
         <v>40</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F32" s="7" t="s">
         <v>75</v>
       </c>
       <c r="G32" s="7"/>
-      <c r="H32" s="18"/>
+      <c r="H32" s="19"/>
       <c r="I32" s="10" t="s">
         <v>87</v>
       </c>
       <c r="J32" s="5"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
     </row>
     <row r="33" spans="1:12" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20"/>
@@ -2102,17 +2081,17 @@
         <v>41</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>46</v>
       </c>
       <c r="G33" s="7"/>
-      <c r="H33" s="18"/>
+      <c r="H33" s="19"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
     </row>
     <row r="34" spans="1:12" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="20"/>
@@ -2124,17 +2103,17 @@
         <v>42</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>46</v>
       </c>
       <c r="G34" s="7"/>
-      <c r="H34" s="18"/>
+      <c r="H34" s="19"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
-      <c r="K34" s="18"/>
-      <c r="L34" s="18"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
     </row>
     <row r="35" spans="1:12" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
@@ -2148,7 +2127,7 @@
         <v>14</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="7" t="s">
@@ -2172,13 +2151,8 @@
       <c r="G36" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K35" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:K35"/>
   <mergeCells count="21">
-    <mergeCell ref="L2:L4"/>
-    <mergeCell ref="L5:L9"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="L14:L26"/>
-    <mergeCell ref="L27:L34"/>
     <mergeCell ref="H14:H26"/>
     <mergeCell ref="K14:K26"/>
     <mergeCell ref="H2:H4"/>
@@ -2195,6 +2169,11 @@
     <mergeCell ref="K2:K4"/>
     <mergeCell ref="K5:K9"/>
     <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="L5:L9"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L14:L26"/>
+    <mergeCell ref="L27:L34"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>